<commit_message>
Update log for CC_Log_2025-05-28.xlsx
</commit_message>
<xml_diff>
--- a/CC_Log_2025-05-28.xlsx
+++ b/CC_Log_2025-05-28.xlsx
@@ -1391,7 +1391,11 @@
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr"/>
       <c r="E78" t="inlineStr"/>
-      <c r="F78" t="inlineStr"/>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>test add 77</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>